<commit_message>
lectura de notas estudiantes de la hoja de calculo con pandas
</commit_message>
<xml_diff>
--- a/sample_data/Aprendizaje-máquina-corte2.xlsx
+++ b/sample_data/Aprendizaje-máquina-corte2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mlcorte2_2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="mlcorte2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="email" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="parcial2" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -422,11 +422,11 @@
   </sheetPr>
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U28" activeCellId="0" sqref="U28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U27" activeCellId="0" sqref="U27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.08"/>
@@ -2292,13 +2292,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.08"/>
@@ -4143,15 +4143,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4166,11 +4161,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4189,11 +4184,11 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
lectura de datos del curso y renderizado del html
</commit_message>
<xml_diff>
--- a/sample_data/Aprendizaje-máquina-corte2.xlsx
+++ b/sample_data/Aprendizaje-máquina-corte2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -320,6 +320,36 @@
   </si>
   <si>
     <t xml:space="preserve">rueda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big data corte 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camilo Rodiguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday 11-13 Wednesday 11-3</t>
   </si>
 </sst>
 </file>
@@ -426,7 +456,7 @@
       <selection pane="topLeft" activeCell="U27" activeCellId="0" sqref="U27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.08"/>
@@ -2298,7 +2328,7 @@
       <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.08"/>
@@ -4159,14 +4189,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4188,7 +4264,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>